<commit_message>
add klasse zu gesamtrangliste
</commit_message>
<xml_diff>
--- a/KWI-RoboChallange_Rangliste_FS2025.xlsx
+++ b/KWI-RoboChallange_Rangliste_FS2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10511"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camillagretsch/KWI-RoboChallenge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB691F0-CA54-4C4B-8F92-B9EABE9EFA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB111CFF-A3C6-834F-83DA-BA2E6E5396A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Linienfolger" sheetId="10" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="61">
   <si>
     <t>Gruppennummer</t>
   </si>
@@ -228,7 +228,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,6 +241,12 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -619,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B79766E1-4E1A-2E4C-A02E-F492E4998716}">
-  <dimension ref="A1:H178"/>
+  <dimension ref="A1:E178"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView topLeftCell="A60" zoomScale="90" workbookViewId="0">
+      <selection activeCell="G79" sqref="G79:H79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1402,7 +1408,7 @@
       </c>
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>65</v>
       </c>
@@ -1414,7 +1420,7 @@
       </c>
       <c r="E65" s="1"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>66</v>
       </c>
@@ -1426,7 +1432,7 @@
       </c>
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>67</v>
       </c>
@@ -1438,7 +1444,7 @@
       </c>
       <c r="E67" s="1"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>68</v>
       </c>
@@ -1450,7 +1456,7 @@
       </c>
       <c r="E68" s="1"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>69</v>
       </c>
@@ -1462,7 +1468,7 @@
       </c>
       <c r="E69" s="1"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>70</v>
       </c>
@@ -1474,7 +1480,7 @@
       </c>
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>71</v>
       </c>
@@ -1486,7 +1492,7 @@
       </c>
       <c r="E71" s="1"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>72</v>
       </c>
@@ -1498,7 +1504,7 @@
       </c>
       <c r="E72" s="1"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>73</v>
       </c>
@@ -1510,7 +1516,7 @@
       </c>
       <c r="E73" s="1"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>74</v>
       </c>
@@ -1522,7 +1528,7 @@
       </c>
       <c r="E74" s="1"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>75</v>
       </c>
@@ -1534,7 +1540,7 @@
       </c>
       <c r="E75" s="1"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>76</v>
       </c>
@@ -1546,7 +1552,7 @@
       </c>
       <c r="E76" s="1"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>77</v>
       </c>
@@ -1558,7 +1564,7 @@
       </c>
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>78</v>
       </c>
@@ -1570,7 +1576,7 @@
       </c>
       <c r="E78" s="1"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>79</v>
       </c>
@@ -1581,15 +1587,8 @@
         <v>7</v>
       </c>
       <c r="E79" s="1"/>
-      <c r="G79">
-        <f>ROUND(H79,2)</f>
-        <v>9.01</v>
-      </c>
-      <c r="H79">
-        <v>9.0060000000000002</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>80</v>
       </c>
@@ -2086,275 +2085,397 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5009128B-BC04-AE43-96E7-DEE798181085}">
-  <dimension ref="A1:A47"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43:B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="B47" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="8809bee8-42c8-488a-8141-8f04d619b36c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1bcd6380-bda3-48d2-8fbc-3eb2b8842e9c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101001FDB85367C20A4499C08F4CA4D5990E0" ma:contentTypeVersion="12" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="f1186bdb3132fe582674e069672a02a8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1bcd6380-bda3-48d2-8fbc-3eb2b8842e9c" xmlns:ns3="8809bee8-42c8-488a-8141-8f04d619b36c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f5a61cc3de785e4f469d070c02522d6" ns2:_="" ns3:_="">
     <xsd:import namespace="1bcd6380-bda3-48d2-8fbc-3eb2b8842e9c"/>
@@ -2555,32 +2676,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C33E82EA-34B8-478E-90E7-7586E722C072}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1bcd6380-bda3-48d2-8fbc-3eb2b8842e9c"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="8809bee8-42c8-488a-8141-8f04d619b36c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64A7263C-2DE4-4511-A0DE-FB7A876B2661}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="8809bee8-42c8-488a-8141-8f04d619b36c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1bcd6380-bda3-48d2-8fbc-3eb2b8842e9c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B06DE4C6-846C-49BD-9837-AEFEE3EFACF3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2598,4 +2714,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64A7263C-2DE4-4511-A0DE-FB7A876B2661}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C33E82EA-34B8-478E-90E7-7586E722C072}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1bcd6380-bda3-48d2-8fbc-3eb2b8842e9c"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="8809bee8-42c8-488a-8141-8f04d619b36c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>